<commit_message>
Update Log In scenarios 10/7/2021
</commit_message>
<xml_diff>
--- a/src/test/java/com/zombieclothing/testData/LogInData_1.xlsx
+++ b/src/test/java/com/zombieclothing/testData/LogInData_1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\ECLIPSE\workspace\zombieClothingV1\src\test\java\com\zombieclothing\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2BF3FB-4FB9-4521-8A13-9095A583C197}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB8C61BC-1CA9-4D64-953F-30E32D3D0CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="-108" windowWidth="22308" windowHeight="13176" xr2:uid="{67A3D090-3389-46D5-B3B6-7B89A24DE821}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>email</t>
   </si>
@@ -42,22 +42,16 @@
     <t>password</t>
   </si>
   <si>
-    <t>abc@gmail.com</t>
-  </si>
-  <si>
-    <t>iqwdnsadas</t>
-  </si>
-  <si>
-    <t>StringHapHap@gmail.com</t>
-  </si>
-  <si>
-    <t>iqwdnsdasds</t>
-  </si>
-  <si>
     <t>vinhtranak02092k@gmail.com</t>
   </si>
   <si>
     <t>Raul1231</t>
+  </si>
+  <si>
+    <t>vinhtranak02092kz@gmail.com</t>
+  </si>
+  <si>
+    <t>Raul123</t>
   </si>
 </sst>
 </file>
@@ -454,7 +448,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -473,33 +467,33 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{386A57CF-7D20-4B2E-9D87-463C7265F90C}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{E99D7743-E1E6-455F-8297-A4DA8289F2F8}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{9DACC7AB-FAB2-4E0C-A1F9-62596704E2F2}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{464A4741-8C9B-43C5-A7B7-C793148BCA3E}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{E84F693A-153D-4C80-AE9E-75EA97AD3227}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>